<commit_message>
phyD FLT hypoxia logfc
</commit_message>
<xml_diff>
--- a/Deep Features via SparseAE/logfc analysis/phyD/hypoxia_phyD_FLT_meta_f.xlsx
+++ b/Deep Features via SparseAE/logfc analysis/phyD/hypoxia_phyD_FLT_meta_f.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LG\Documents\NASA_GeneLab\Deep Features via SparseAE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LG\Documents\NASA_GeneLab\Deep Features via SparseAE\logfc analysis\phyD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC55110E-4DC7-40E4-B2B4-723A91A29DDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8814EF-BBE0-417A-8110-4B6B171EB30E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F3E799CD-3372-4495-B935-8B20C90FC233}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1841" uniqueCount="1560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="1561">
   <si>
     <t>TAIR</t>
   </si>
@@ -4714,6 +4714,10 @@
   </si>
   <si>
     <t>3702.ATMG01190.1</t>
+  </si>
+  <si>
+    <t>APR2.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -5082,8 +5086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF2C7E1-3E2E-4C0F-B117-DCC07118BACC}">
   <dimension ref="A1:G309"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6489,8 +6493,8 @@
       <c r="A62" t="s">
         <v>310</v>
       </c>
-      <c r="B62" s="1">
-        <v>44288</v>
+      <c r="B62" s="1" t="s">
+        <v>1560</v>
       </c>
       <c r="C62" t="s">
         <v>311</v>

</xml_diff>